<commit_message>
Updated the slides and initial plan with a sketched schedule
</commit_message>
<xml_diff>
--- a/doc/gantt.xlsx
+++ b/doc/gantt.xlsx
@@ -142,6 +142,113 @@
         <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Start Date</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>42449.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42463.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42477.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42491.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42505.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42519.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Duration</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:alpha val="90000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
@@ -259,11 +366,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2128950536"/>
-        <c:axId val="2127952168"/>
+        <c:axId val="2111113864"/>
+        <c:axId val="2111117192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2128950536"/>
+        <c:axId val="2111113864"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -272,19 +379,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2127952168"/>
+        <c:crossAx val="2111117192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -292,7 +387,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127952168"/>
+        <c:axId val="2111117192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42535.0"/>
@@ -308,28 +403,36 @@
         <c:spPr>
           <a:effectLst/>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2128950536"/>
+        <c:crossAx val="2111113864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="15.0"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+      </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:noFill/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -344,14 +447,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>